<commit_message>
Roll back các file excel để fix lỗi
</commit_message>
<xml_diff>
--- a/jyx2/Assets/Mods/JYX2/Configs/战斗.xlsx
+++ b/jyx2/Assets/Mods/JYX2/Configs/战斗.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/WorkSpace/unity/_project/jynew/jyx2/Assets/Mods/JYX2/Configs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\jynew\jyx2\Assets\Mods\JYX2\Configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEA73E2-B18C-8641-884A-6F5E9B2115EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FB77AB-43B6-4380-B0EC-9DDDB68572DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="1880" windowWidth="19140" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="1870" windowWidth="19140" windowHeight="13090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="战斗数据" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,404 @@
     <t>音乐</t>
   </si>
   <si>
+    <t>明教分舵</t>
+  </si>
+  <si>
+    <t>光明左使</t>
+  </si>
+  <si>
+    <t>徐降莫大</t>
+  </si>
+  <si>
+    <t>徐降左</t>
+  </si>
+  <si>
+    <t>令降莫大</t>
+  </si>
+  <si>
+    <t>令降左</t>
+  </si>
+  <si>
+    <t>青城四秀</t>
+  </si>
+  <si>
+    <t>笑傲江湖</t>
+  </si>
+  <si>
+    <t>凌霄城外</t>
+  </si>
+  <si>
+    <t>蜘蛛洞一</t>
+  </si>
+  <si>
+    <t>蜘蛛洞二</t>
+  </si>
+  <si>
+    <t>蜘蛛洞三</t>
+  </si>
+  <si>
+    <t>蜘蛛洞四</t>
+  </si>
+  <si>
+    <t>蜘蛛洞五</t>
+  </si>
+  <si>
+    <t>救神鵰</t>
+  </si>
+  <si>
+    <t>少林寺外</t>
+  </si>
+  <si>
+    <t>救阿紫</t>
+  </si>
+  <si>
+    <t>十大善人</t>
+  </si>
+  <si>
+    <t>斗胡斐</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>中阎基计</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>杀阎基</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>救苗人凤</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>胡苗对决</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>闯王宝藏</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>成昆奸计</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>光明顶前</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>决战六派</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>弒杀成昆</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>救王难姑</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>光明圣火</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>会七伤拳</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>闹崆峒</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>救庸医</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>闹昆仑</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>夺倚天剑</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>峨嵋围攻</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>三丰指导</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>闯见性峰</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗定闲</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗泰山</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗天门</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>闯衡山</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗莫大</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>闯嵩山</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>徐降天门</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>徐降定闲</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>令降天门</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>令降定闲</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>再斗嵩山</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>再斗定闲</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>再斗天门</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>再斗莫大</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>杀费彬</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗丹青生</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗秃笔翁</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗黑白子</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗黄钟公</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗四友</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗林平之</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗余沧海</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>平之复仇</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗平一指</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>杀田伯光</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>东方不败</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>葵花宝典</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>任与东方</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗白万剑</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>战雪山派</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>战老顽童</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>杀一灯</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>战欧阳克</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁掌帮外</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>战裘千仞</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>再战铁掌</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>闯重阳宫</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>战丘处机</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>再战全真</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>挑战郭靖</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>战桃花岛</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>解剑岩前</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>战玄慈</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>破打狗阵</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>单挑乔峰</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>丐帮四老</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>慕容奸计</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>杀丁春秋</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>战游坦之</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>闯鳄鱼潭</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗岳老三</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>大轮寺外</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>大轮寺内</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>抢连城诀</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>闯神龙岛</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗洪教主</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>闯五毒教</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>找韦小宝</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗蓝凤凰</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>闯金轮寺</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>斗金轮王</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>战袁承志</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>大会斗唐</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>再斗金花</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>十大恶人</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>无用</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>Exp</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -529,6 +927,14 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>千年人参</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>莽牯朱蛤</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>251,252,253,254</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -578,412 +984,6 @@
   </si>
   <si>
     <t>0,1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Đậu Hồ Phi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trung Nham Jiji</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Giết Yến Cơ</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cứu Miao Renfeng</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cuộc đọ sức giữa Hồ và Miêu</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nhân sâm thiên niên kỷ</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Kho báu Chuangwang</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>chi nhánh minh giao</t>
-  </si>
-  <si>
-    <t>Sứ giả ánh sáng</t>
-  </si>
-  <si>
-    <t>Âm mưu của Trình Côn</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Đối diện Quảng Minh Định</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trận chiến quyết định giữa sáu phe</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Giết Thành Côn</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cứu Vương Nam Cốc</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ngọn lửa thiêng sáng ngời</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Biết Bảy Chấn Thương Quyền Anh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nao Kongtong</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lưu lại sự lang băm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ồn ào ở Côn Lôn</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Giành lấy Thiên kiếm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cuộc vây hãm Nga Mi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mitutoyo hướng dẫn</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Chongjianxingfeng</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Đậu Định Tiên</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Núi Tài</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Đấu Thiên Môn</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tới núi Hằng Sơn</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Đậu Mộ Đa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trang Tùng Sơn</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Từ Giang Thiên Môn</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hứa Giang Đỉnh Tiên</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hứa Giang Mộ Đa</t>
-  </si>
-  <si>
-    <t>Từ Giang Tả</t>
-  </si>
-  <si>
-    <t>Lệnh xuống Thiên Môn</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ra lệnh ổn định</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Đơn hàng rất lớn</t>
-  </si>
-  <si>
-    <t>Đặt hàng Jiangzuo</t>
-  </si>
-  <si>
-    <t>Chiến đấu với Songshan một lần nữa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hãy chiến đấu một lần nữa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Chiến đấu với Thiên Môn lần nữa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sẽ thật tuyệt nếu chúng ta chiến đấu một lần nữa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Giết Phi Bân</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Đan Thanh Sinh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Đậu Tubi Weng</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>chiến đấu đen trắng</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Đỗ Hoàng Trung Công</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Đỗ Tư Hữu</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Đậu Lâm Bình Chi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Thanh Thành Bốn Chương Trình</t>
-  </si>
-  <si>
-    <t>Đỗ Vũ Thương Hải</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sự trả thù của Ping</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Một ngón tay</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Giết Điền Bá Quang</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Phương Đông bất bại</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bộ sưu tập hướng dương</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Người đánh kiếm</t>
-  </si>
-  <si>
-    <t>Nhân và Đông Phương</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bên ngoài thành phố Lingxiao</t>
-  </si>
-  <si>
-    <t>Đỗ Bạch Vạn Kiếm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Chiến đấu với giáo phái Núi Tuyết</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hang Nhện Một</t>
-  </si>
-  <si>
-    <t>Hang Nhện 2</t>
-  </si>
-  <si>
-    <t>Hang Nhện Ba</t>
-  </si>
-  <si>
-    <t>Hang Nhện Bốn</t>
-  </si>
-  <si>
-    <t>hang nhện năm</t>
-  </si>
-  <si>
-    <t>cứu đại bàng</t>
-  </si>
-  <si>
-    <t>Chiến tranh với cậu bé già nghịch ngợm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Giết một chiếc đèn</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Triển Âu Dương Khả</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bên ngoài Gang Palm Gang</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Triển Thu Thiên Nhân</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Chiến đấu với cây cọ sắt lần nữa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bước vào cung điện Sùng Dương</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Zhanqiu Chuji</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Đánh Tuyền Chân lần nữa</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Thử thách Quách Tĩnh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trận chiến trên đảo hoa đào</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ngao đỏ Manggu</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jie Jian Yan Qian</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bên ngoài chùa Thiếu Lâm</t>
-  </si>
-  <si>
-    <t>Triển Huyền Từ</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Phá vỡ đội hình chó</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Thử thách Kiều Phong</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bốn trưởng lão của tộc ăn xin</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Âm mưu thâm độc của Mộ Dung</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Giết Đinh Xuân Thu</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cứu A Tử</t>
-  </si>
-  <si>
-    <t>Zhan Youtanzhi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Vào ao cá sấu</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Đậu Nhạc Lão San</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bên ngoài chùa Dalunji</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bên trong chùa Dalinji</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bí quyết chiếm thành phố</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Đột nhập vào đảo Thần Long</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Chúa Douhong</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Đột nhập vào Ngũ Độc Giáo</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Đi tìm Vi Tiểu Bảo</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Phượng Hoàng Đấu Lan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Tham quan chùa Jinlun</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Doujinlunwang</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Zhan Yuan Chengzhi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quốc hội đấu tranh chống nhà Đường</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Một cuộc chiến khác với hoa vàng</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mười nhân vật phản diện hàng đầu</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mười người tốt nhất</t>
-  </si>
-  <si>
-    <t>vô ích</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -991,7 +991,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1046,7 +1046,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1326,26 +1326,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B144"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.6328125" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" customWidth="1"/>
     <col min="8" max="8" width="91" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>237</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="14">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1362,76 +1362,76 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>74</v>
+        <v>178</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>115</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="14">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>132</v>
+        <v>238</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>134</v>
+        <v>240</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>134</v>
+        <v>240</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>132</v>
+        <v>238</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>132</v>
+        <v>238</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>133</v>
+        <v>239</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>133</v>
+        <v>239</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>112</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>110</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>114</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>116</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>141</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>186</v>
       </c>
       <c r="D5">
         <v>150</v>
@@ -1449,15 +1449,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>187</v>
       </c>
       <c r="D6">
         <v>200</v>
@@ -1475,15 +1475,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>191</v>
       </c>
       <c r="D7">
         <v>100</v>
@@ -1492,7 +1492,7 @@
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>140</v>
+        <v>246</v>
       </c>
       <c r="G7">
         <v>-1</v>
@@ -1501,15 +1501,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>192</v>
       </c>
       <c r="D8">
         <v>100</v>
@@ -1524,18 +1524,18 @@
         <v>-1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>193</v>
       </c>
       <c r="D9">
         <v>500</v>
@@ -1553,15 +1553,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="14">
+    <row r="10" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>146</v>
+        <v>232</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>194</v>
       </c>
       <c r="D10">
         <v>500</v>
@@ -1576,18 +1576,18 @@
         <v>-1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>147</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>194</v>
       </c>
       <c r="D11">
         <v>1000</v>
@@ -1602,18 +1602,18 @@
         <v>-1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>141</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>186</v>
       </c>
       <c r="D12">
         <v>50</v>
@@ -1631,15 +1631,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>148</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>195</v>
       </c>
       <c r="D13">
         <v>300</v>
@@ -1654,18 +1654,18 @@
         <v>-1</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>149</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>195</v>
       </c>
       <c r="D14">
         <v>500</v>
@@ -1680,18 +1680,18 @@
         <v>-1</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>150</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>195</v>
       </c>
       <c r="D15">
         <v>400</v>
@@ -1709,15 +1709,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>151</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>196</v>
       </c>
       <c r="D16">
         <v>800</v>
@@ -1732,18 +1732,18 @@
         <v>-1</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>152</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>108</v>
+        <v>212</v>
       </c>
       <c r="D17">
         <v>2300</v>
@@ -1758,18 +1758,18 @@
         <v>-1</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>153</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>109</v>
+        <v>213</v>
       </c>
       <c r="D18">
         <v>2000</v>
@@ -1784,18 +1784,18 @@
         <v>-1</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>154</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>110</v>
+        <v>214</v>
       </c>
       <c r="D19">
         <v>400</v>
@@ -1813,15 +1813,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>155</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>111</v>
+        <v>215</v>
       </c>
       <c r="D20">
         <v>2000</v>
@@ -1836,18 +1836,18 @@
         <v>-1</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>156</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>112</v>
+        <v>216</v>
       </c>
       <c r="D21">
         <v>400</v>
@@ -1862,18 +1862,18 @@
         <v>-1</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>157</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>198</v>
       </c>
       <c r="D22">
         <v>200</v>
@@ -1888,18 +1888,18 @@
         <v>-1</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>158</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>196</v>
       </c>
       <c r="D23">
         <v>400</v>
@@ -1914,18 +1914,18 @@
         <v>-1</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>159</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>112</v>
+        <v>216</v>
       </c>
       <c r="D24">
         <v>400</v>
@@ -1940,18 +1940,18 @@
         <v>-1</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>160</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>217</v>
       </c>
       <c r="D25">
         <v>800</v>
@@ -1969,15 +1969,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>161</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>114</v>
+        <v>218</v>
       </c>
       <c r="D26">
         <v>300</v>
@@ -1992,18 +1992,18 @@
         <v>-1</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>162</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>115</v>
+        <v>219</v>
       </c>
       <c r="D27">
         <v>3000</v>
@@ -2021,15 +2021,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>163</v>
+        <v>42</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>182</v>
       </c>
       <c r="D28">
         <v>200</v>
@@ -2044,18 +2044,18 @@
         <v>-1</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D29">
         <v>500</v>
@@ -2070,18 +2070,18 @@
         <v>-1</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>165</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
-        <v>116</v>
+        <v>220</v>
       </c>
       <c r="D30">
         <v>200</v>
@@ -2096,18 +2096,18 @@
         <v>-1</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>166</v>
+        <v>45</v>
       </c>
       <c r="C31" t="s">
-        <v>116</v>
+        <v>220</v>
       </c>
       <c r="D31">
         <v>500</v>
@@ -2122,18 +2122,18 @@
         <v>-1</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>167</v>
+        <v>46</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>198</v>
       </c>
       <c r="D32">
         <v>200</v>
@@ -2148,18 +2148,18 @@
         <v>-1</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>168</v>
+        <v>47</v>
       </c>
       <c r="C33" t="s">
-        <v>112</v>
+        <v>216</v>
       </c>
       <c r="D33">
         <v>500</v>
@@ -2174,18 +2174,18 @@
         <v>-1</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>169</v>
+        <v>48</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>181</v>
       </c>
       <c r="D34">
         <v>200</v>
@@ -2200,18 +2200,18 @@
         <v>-1</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>170</v>
+        <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>181</v>
       </c>
       <c r="D35">
         <v>500</v>
@@ -2229,15 +2229,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>171</v>
+        <v>50</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D36">
         <v>500</v>
@@ -2255,15 +2255,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>172</v>
+        <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D37">
         <v>500</v>
@@ -2281,15 +2281,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>173</v>
+        <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D38">
         <v>800</v>
@@ -2307,15 +2307,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>174</v>
+        <v>51</v>
       </c>
       <c r="C39" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D39">
         <v>500</v>
@@ -2333,15 +2333,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>175</v>
+        <v>52</v>
       </c>
       <c r="C40" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D40">
         <v>500</v>
@@ -2359,15 +2359,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>36</v>
       </c>
       <c r="B41" t="s">
-        <v>176</v>
+        <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>77</v>
+        <v>181</v>
       </c>
       <c r="D41">
         <v>500</v>
@@ -2385,15 +2385,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>37</v>
       </c>
       <c r="B42" t="s">
-        <v>177</v>
+        <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D42">
         <v>800</v>
@@ -2411,15 +2411,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>38</v>
       </c>
       <c r="B43" t="s">
-        <v>178</v>
+        <v>53</v>
       </c>
       <c r="C43" t="s">
-        <v>78</v>
+        <v>182</v>
       </c>
       <c r="D43">
         <v>400</v>
@@ -2434,18 +2434,18 @@
         <v>-1</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>39</v>
       </c>
       <c r="B44" t="s">
-        <v>179</v>
+        <v>54</v>
       </c>
       <c r="C44" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D44">
         <v>200</v>
@@ -2460,18 +2460,18 @@
         <v>-1</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>180</v>
+        <v>55</v>
       </c>
       <c r="C45" t="s">
-        <v>116</v>
+        <v>220</v>
       </c>
       <c r="D45">
         <v>200</v>
@@ -2486,18 +2486,18 @@
         <v>-1</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>41</v>
       </c>
       <c r="B46" t="s">
-        <v>181</v>
+        <v>56</v>
       </c>
       <c r="C46" t="s">
-        <v>94</v>
+        <v>198</v>
       </c>
       <c r="D46">
         <v>200</v>
@@ -2512,18 +2512,18 @@
         <v>-1</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>42</v>
       </c>
       <c r="B47" t="s">
-        <v>182</v>
+        <v>57</v>
       </c>
       <c r="C47" t="s">
-        <v>112</v>
+        <v>216</v>
       </c>
       <c r="D47">
         <v>100</v>
@@ -2538,18 +2538,18 @@
         <v>-1</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>43</v>
       </c>
       <c r="B48" t="s">
-        <v>183</v>
+        <v>58</v>
       </c>
       <c r="C48" t="s">
-        <v>126</v>
+        <v>230</v>
       </c>
       <c r="D48">
         <v>300</v>
@@ -2567,15 +2567,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>44</v>
       </c>
       <c r="B49" t="s">
-        <v>184</v>
+        <v>59</v>
       </c>
       <c r="C49" t="s">
-        <v>124</v>
+        <v>228</v>
       </c>
       <c r="D49">
         <v>400</v>
@@ -2593,15 +2593,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>45</v>
       </c>
       <c r="B50" t="s">
-        <v>185</v>
+        <v>60</v>
       </c>
       <c r="C50" t="s">
-        <v>125</v>
+        <v>229</v>
       </c>
       <c r="D50">
         <v>500</v>
@@ -2619,15 +2619,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>46</v>
       </c>
       <c r="B51" t="s">
-        <v>186</v>
+        <v>61</v>
       </c>
       <c r="C51" t="s">
-        <v>124</v>
+        <v>228</v>
       </c>
       <c r="D51">
         <v>600</v>
@@ -2645,15 +2645,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>47</v>
       </c>
       <c r="B52" t="s">
-        <v>187</v>
+        <v>62</v>
       </c>
       <c r="C52" t="s">
-        <v>124</v>
+        <v>228</v>
       </c>
       <c r="D52">
         <v>1200</v>
@@ -2668,18 +2668,18 @@
         <v>-1</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>48</v>
       </c>
       <c r="B53" t="s">
-        <v>188</v>
+        <v>63</v>
       </c>
       <c r="C53" t="s">
-        <v>94</v>
+        <v>198</v>
       </c>
       <c r="D53">
         <v>50</v>
@@ -2697,15 +2697,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>49</v>
       </c>
       <c r="B54" t="s">
-        <v>189</v>
+        <v>11</v>
       </c>
       <c r="C54" t="s">
-        <v>123</v>
+        <v>227</v>
       </c>
       <c r="D54">
         <v>200</v>
@@ -2720,18 +2720,18 @@
         <v>-1</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>50</v>
       </c>
       <c r="B55" t="s">
-        <v>190</v>
+        <v>64</v>
       </c>
       <c r="C55" t="s">
-        <v>123</v>
+        <v>227</v>
       </c>
       <c r="D55">
         <v>500</v>
@@ -2746,18 +2746,18 @@
         <v>-1</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>51</v>
       </c>
       <c r="B56" t="s">
-        <v>191</v>
+        <v>65</v>
       </c>
       <c r="C56" t="s">
-        <v>123</v>
+        <v>227</v>
       </c>
       <c r="D56">
         <v>500</v>
@@ -2772,18 +2772,18 @@
         <v>36</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>52</v>
       </c>
       <c r="B57" t="s">
-        <v>192</v>
+        <v>66</v>
       </c>
       <c r="C57" t="s">
-        <v>89</v>
+        <v>193</v>
       </c>
       <c r="D57">
         <v>50</v>
@@ -2801,15 +2801,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>53</v>
       </c>
       <c r="B58" t="s">
-        <v>193</v>
+        <v>67</v>
       </c>
       <c r="C58" t="s">
-        <v>94</v>
+        <v>198</v>
       </c>
       <c r="D58">
         <v>450</v>
@@ -2827,15 +2827,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>54</v>
       </c>
       <c r="B59" t="s">
-        <v>194</v>
+        <v>68</v>
       </c>
       <c r="C59" t="s">
-        <v>122</v>
+        <v>226</v>
       </c>
       <c r="D59">
         <v>5000</v>
@@ -2850,18 +2850,18 @@
         <v>-1</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>55</v>
       </c>
       <c r="B60" t="s">
-        <v>195</v>
+        <v>69</v>
       </c>
       <c r="C60" t="s">
-        <v>121</v>
+        <v>225</v>
       </c>
       <c r="D60">
         <v>2000</v>
@@ -2876,18 +2876,18 @@
         <v>-1</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>56</v>
       </c>
       <c r="B61" t="s">
-        <v>196</v>
+        <v>12</v>
       </c>
       <c r="C61" t="s">
-        <v>121</v>
+        <v>225</v>
       </c>
       <c r="D61">
         <v>2500</v>
@@ -2902,18 +2902,18 @@
         <v>-1</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>57</v>
       </c>
       <c r="B62" t="s">
-        <v>197</v>
+        <v>70</v>
       </c>
       <c r="C62" t="s">
-        <v>121</v>
+        <v>225</v>
       </c>
       <c r="D62">
         <v>5000</v>
@@ -2922,24 +2922,24 @@
         <v>7</v>
       </c>
       <c r="F62" t="s">
-        <v>75</v>
+        <v>179</v>
       </c>
       <c r="G62">
         <v>-1</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>58</v>
       </c>
       <c r="B63" t="s">
-        <v>198</v>
+        <v>13</v>
       </c>
       <c r="C63" t="s">
-        <v>119</v>
+        <v>223</v>
       </c>
       <c r="D63">
         <v>100</v>
@@ -2954,18 +2954,18 @@
         <v>-1</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>59</v>
       </c>
       <c r="B64" t="s">
-        <v>199</v>
+        <v>71</v>
       </c>
       <c r="C64" t="s">
-        <v>120</v>
+        <v>224</v>
       </c>
       <c r="D64">
         <v>200</v>
@@ -2983,15 +2983,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>60</v>
       </c>
       <c r="B65" t="s">
-        <v>200</v>
+        <v>72</v>
       </c>
       <c r="C65" t="s">
-        <v>119</v>
+        <v>223</v>
       </c>
       <c r="D65">
         <v>300</v>
@@ -3006,18 +3006,18 @@
         <v>-1</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>201</v>
+        <v>14</v>
       </c>
       <c r="C66" t="s">
-        <v>118</v>
+        <v>222</v>
       </c>
       <c r="D66">
         <v>280</v>
@@ -3032,18 +3032,18 @@
         <v>-1</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>62</v>
       </c>
       <c r="B67" t="s">
-        <v>202</v>
+        <v>15</v>
       </c>
       <c r="C67" t="s">
-        <v>118</v>
+        <v>222</v>
       </c>
       <c r="D67">
         <v>280</v>
@@ -3058,18 +3058,18 @@
         <v>-1</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>63</v>
       </c>
       <c r="B68" t="s">
-        <v>203</v>
+        <v>16</v>
       </c>
       <c r="C68" t="s">
-        <v>118</v>
+        <v>222</v>
       </c>
       <c r="D68">
         <v>630</v>
@@ -3084,18 +3084,18 @@
         <v>-1</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>64</v>
       </c>
       <c r="B69" t="s">
-        <v>204</v>
+        <v>17</v>
       </c>
       <c r="C69" t="s">
-        <v>118</v>
+        <v>222</v>
       </c>
       <c r="D69">
         <v>280</v>
@@ -3110,18 +3110,18 @@
         <v>-1</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>65</v>
       </c>
       <c r="B70" t="s">
-        <v>205</v>
+        <v>18</v>
       </c>
       <c r="C70" t="s">
-        <v>118</v>
+        <v>222</v>
       </c>
       <c r="D70">
         <v>280</v>
@@ -3136,18 +3136,18 @@
         <v>-1</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>66</v>
       </c>
       <c r="B71" t="s">
-        <v>206</v>
+        <v>19</v>
       </c>
       <c r="C71" t="s">
-        <v>117</v>
+        <v>221</v>
       </c>
       <c r="D71">
         <v>950</v>
@@ -3165,15 +3165,15 @@
         <v>77</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>67</v>
       </c>
       <c r="B72" t="s">
-        <v>207</v>
+        <v>73</v>
       </c>
       <c r="C72" t="s">
-        <v>79</v>
+        <v>183</v>
       </c>
       <c r="D72">
         <v>1500</v>
@@ -3191,15 +3191,15 @@
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>68</v>
       </c>
       <c r="B73" t="s">
-        <v>208</v>
+        <v>74</v>
       </c>
       <c r="C73" t="s">
-        <v>87</v>
+        <v>191</v>
       </c>
       <c r="D73">
         <v>1500</v>
@@ -3217,15 +3217,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>69</v>
       </c>
       <c r="B74" t="s">
-        <v>209</v>
+        <v>75</v>
       </c>
       <c r="C74" t="s">
-        <v>112</v>
+        <v>216</v>
       </c>
       <c r="D74">
         <v>300</v>
@@ -3243,15 +3243,15 @@
         <v>61</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>70</v>
       </c>
       <c r="B75" t="s">
-        <v>210</v>
+        <v>76</v>
       </c>
       <c r="C75" t="s">
-        <v>81</v>
+        <v>185</v>
       </c>
       <c r="D75">
         <v>300</v>
@@ -3266,18 +3266,18 @@
         <v>-1</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>71</v>
       </c>
       <c r="B76" t="s">
-        <v>211</v>
+        <v>77</v>
       </c>
       <c r="C76" t="s">
-        <v>81</v>
+        <v>185</v>
       </c>
       <c r="D76">
         <v>1600</v>
@@ -3292,18 +3292,18 @@
         <v>-1</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>72</v>
       </c>
       <c r="B77" t="s">
-        <v>212</v>
+        <v>78</v>
       </c>
       <c r="C77" t="s">
-        <v>81</v>
+        <v>185</v>
       </c>
       <c r="D77">
         <v>900</v>
@@ -3318,18 +3318,18 @@
         <v>-1</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>73</v>
       </c>
       <c r="B78" t="s">
-        <v>213</v>
+        <v>79</v>
       </c>
       <c r="C78" t="s">
-        <v>81</v>
+        <v>185</v>
       </c>
       <c r="D78">
         <v>330</v>
@@ -3344,18 +3344,18 @@
         <v>-1</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>74</v>
       </c>
       <c r="B79" t="s">
+        <v>80</v>
+      </c>
+      <c r="C79" t="s">
         <v>214</v>
-      </c>
-      <c r="C79" t="s">
-        <v>110</v>
       </c>
       <c r="D79">
         <v>1650</v>
@@ -3370,18 +3370,18 @@
         <v>-1</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>75</v>
       </c>
       <c r="B80" t="s">
-        <v>215</v>
+        <v>81</v>
       </c>
       <c r="C80" t="s">
-        <v>110</v>
+        <v>214</v>
       </c>
       <c r="D80">
         <v>850</v>
@@ -3396,18 +3396,18 @@
         <v>-1</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>76</v>
       </c>
       <c r="B81" t="s">
-        <v>216</v>
+        <v>82</v>
       </c>
       <c r="C81" t="s">
-        <v>107</v>
+        <v>211</v>
       </c>
       <c r="D81">
         <v>1500</v>
@@ -3425,15 +3425,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>77</v>
       </c>
       <c r="B82" t="s">
-        <v>217</v>
+        <v>83</v>
       </c>
       <c r="C82" t="s">
-        <v>79</v>
+        <v>183</v>
       </c>
       <c r="D82">
         <v>2300</v>
@@ -3448,18 +3448,18 @@
         <v>-1</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="14">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="13" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>78</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>218</v>
+        <v>233</v>
       </c>
       <c r="C83" t="s">
-        <v>106</v>
+        <v>210</v>
       </c>
       <c r="D83">
         <v>600</v>
@@ -3477,15 +3477,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>79</v>
       </c>
       <c r="B84" t="s">
-        <v>219</v>
+        <v>84</v>
       </c>
       <c r="C84" t="s">
-        <v>105</v>
+        <v>209</v>
       </c>
       <c r="D84">
         <v>400</v>
@@ -3500,18 +3500,18 @@
         <v>-1</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>80</v>
       </c>
       <c r="B85" t="s">
-        <v>220</v>
+        <v>20</v>
       </c>
       <c r="C85" t="s">
-        <v>104</v>
+        <v>208</v>
       </c>
       <c r="D85">
         <v>600</v>
@@ -3526,18 +3526,18 @@
         <v>-1</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>81</v>
       </c>
       <c r="B86" t="s">
-        <v>221</v>
+        <v>85</v>
       </c>
       <c r="C86" t="s">
-        <v>104</v>
+        <v>208</v>
       </c>
       <c r="D86">
         <v>1500</v>
@@ -3552,18 +3552,18 @@
         <v>-1</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>82</v>
       </c>
       <c r="B87" t="s">
-        <v>222</v>
+        <v>86</v>
       </c>
       <c r="C87" t="s">
-        <v>103</v>
+        <v>207</v>
       </c>
       <c r="D87">
         <v>600</v>
@@ -3578,18 +3578,18 @@
         <v>-1</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>83</v>
       </c>
       <c r="B88" t="s">
-        <v>223</v>
+        <v>87</v>
       </c>
       <c r="C88" t="s">
-        <v>103</v>
+        <v>207</v>
       </c>
       <c r="D88">
         <v>1800</v>
@@ -3607,15 +3607,15 @@
         <v>50</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>84</v>
       </c>
       <c r="B89" t="s">
-        <v>224</v>
+        <v>88</v>
       </c>
       <c r="C89" t="s">
-        <v>98</v>
+        <v>202</v>
       </c>
       <c r="D89">
         <v>1000</v>
@@ -3630,18 +3630,18 @@
         <v>-1</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>85</v>
       </c>
       <c r="B90" t="s">
-        <v>225</v>
+        <v>89</v>
       </c>
       <c r="C90" t="s">
-        <v>98</v>
+        <v>202</v>
       </c>
       <c r="D90">
         <v>500</v>
@@ -3659,15 +3659,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>86</v>
       </c>
       <c r="B91" t="s">
-        <v>226</v>
+        <v>90</v>
       </c>
       <c r="C91" t="s">
-        <v>102</v>
+        <v>206</v>
       </c>
       <c r="D91">
         <v>1300</v>
@@ -3682,18 +3682,18 @@
         <v>-1</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>87</v>
       </c>
       <c r="B92" t="s">
-        <v>227</v>
+        <v>21</v>
       </c>
       <c r="C92" t="s">
-        <v>97</v>
+        <v>201</v>
       </c>
       <c r="D92">
         <v>200</v>
@@ -3708,18 +3708,18 @@
         <v>-1</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>88</v>
       </c>
       <c r="B93" t="s">
-        <v>228</v>
+        <v>91</v>
       </c>
       <c r="C93" t="s">
-        <v>101</v>
+        <v>205</v>
       </c>
       <c r="D93">
         <v>700</v>
@@ -3737,15 +3737,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>89</v>
       </c>
       <c r="B94" t="s">
-        <v>229</v>
+        <v>92</v>
       </c>
       <c r="C94" t="s">
-        <v>100</v>
+        <v>204</v>
       </c>
       <c r="D94">
         <v>900</v>
@@ -3760,18 +3760,18 @@
         <v>-1</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>90</v>
       </c>
       <c r="B95" t="s">
-        <v>230</v>
+        <v>93</v>
       </c>
       <c r="C95" t="s">
-        <v>99</v>
+        <v>203</v>
       </c>
       <c r="D95">
         <v>2400</v>
@@ -3786,18 +3786,18 @@
         <v>-1</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>91</v>
       </c>
       <c r="B96" t="s">
-        <v>231</v>
+        <v>94</v>
       </c>
       <c r="C96" t="s">
-        <v>98</v>
+        <v>202</v>
       </c>
       <c r="D96">
         <v>300</v>
@@ -3812,18 +3812,18 @@
         <v>-1</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>92</v>
       </c>
       <c r="B97" t="s">
-        <v>232</v>
+        <v>95</v>
       </c>
       <c r="C97" t="s">
-        <v>97</v>
+        <v>201</v>
       </c>
       <c r="D97">
         <v>500</v>
@@ -3838,18 +3838,18 @@
         <v>-1</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>93</v>
       </c>
       <c r="B98" t="s">
-        <v>233</v>
+        <v>96</v>
       </c>
       <c r="C98" t="s">
-        <v>96</v>
+        <v>200</v>
       </c>
       <c r="D98">
         <v>1500</v>
@@ -3864,18 +3864,18 @@
         <v>-1</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>94</v>
       </c>
       <c r="B99" t="s">
-        <v>234</v>
+        <v>97</v>
       </c>
       <c r="C99" t="s">
-        <v>94</v>
+        <v>198</v>
       </c>
       <c r="D99">
         <v>550</v>
@@ -3890,18 +3890,18 @@
         <v>-1</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>95</v>
       </c>
       <c r="B100" t="s">
-        <v>235</v>
+        <v>98</v>
       </c>
       <c r="C100" t="s">
-        <v>94</v>
+        <v>198</v>
       </c>
       <c r="D100">
         <v>1000</v>
@@ -3916,18 +3916,18 @@
         <v>-1</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>96</v>
       </c>
       <c r="B101" t="s">
-        <v>236</v>
+        <v>99</v>
       </c>
       <c r="C101" t="s">
-        <v>95</v>
+        <v>199</v>
       </c>
       <c r="D101">
         <v>230</v>
@@ -3942,18 +3942,18 @@
         <v>-1</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>97</v>
       </c>
       <c r="B102" t="s">
-        <v>237</v>
+        <v>100</v>
       </c>
       <c r="C102" t="s">
-        <v>83</v>
+        <v>187</v>
       </c>
       <c r="D102">
         <v>350</v>
@@ -3968,18 +3968,18 @@
         <v>-1</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>98</v>
       </c>
       <c r="B103" t="s">
-        <v>238</v>
+        <v>101</v>
       </c>
       <c r="C103" t="s">
-        <v>87</v>
+        <v>191</v>
       </c>
       <c r="D103">
         <v>850</v>
@@ -3994,18 +3994,18 @@
         <v>-1</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>99</v>
       </c>
       <c r="B104" t="s">
-        <v>239</v>
+        <v>102</v>
       </c>
       <c r="C104" t="s">
-        <v>94</v>
+        <v>198</v>
       </c>
       <c r="D104">
         <v>450</v>
@@ -4020,18 +4020,18 @@
         <v>-1</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>100</v>
       </c>
       <c r="B105" t="s">
-        <v>240</v>
+        <v>103</v>
       </c>
       <c r="C105" t="s">
-        <v>93</v>
+        <v>197</v>
       </c>
       <c r="D105">
         <v>1250</v>
@@ -4046,18 +4046,18 @@
         <v>-1</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>101</v>
       </c>
       <c r="B106" t="s">
-        <v>241</v>
+        <v>104</v>
       </c>
       <c r="C106" t="s">
-        <v>87</v>
+        <v>191</v>
       </c>
       <c r="D106">
         <v>600</v>
@@ -4075,15 +4075,15 @@
         <v>54</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>102</v>
       </c>
       <c r="B107" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C107" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D107">
         <v>500</v>
@@ -4101,15 +4101,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>103</v>
       </c>
       <c r="B108" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C108" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D108">
         <v>600</v>
@@ -4127,15 +4127,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>104</v>
       </c>
       <c r="B109" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C109" t="s">
-        <v>77</v>
+        <v>181</v>
       </c>
       <c r="D109">
         <v>700</v>
@@ -4153,15 +4153,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>105</v>
       </c>
       <c r="B110" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C110" t="s">
-        <v>78</v>
+        <v>182</v>
       </c>
       <c r="D110">
         <v>800</v>
@@ -4179,15 +4179,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>106</v>
       </c>
       <c r="B111" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C111" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D111">
         <v>900</v>
@@ -4205,15 +4205,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>107</v>
       </c>
       <c r="B112" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C112" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D112">
         <v>1000</v>
@@ -4231,15 +4231,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>108</v>
       </c>
       <c r="B113" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C113" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D113">
         <v>1100</v>
@@ -4257,15 +4257,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>109</v>
       </c>
       <c r="B114" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C114" t="s">
-        <v>77</v>
+        <v>181</v>
       </c>
       <c r="D114">
         <v>1200</v>
@@ -4283,15 +4283,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>110</v>
       </c>
       <c r="B115" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C115" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D115">
         <v>1300</v>
@@ -4309,15 +4309,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>111</v>
       </c>
       <c r="B116" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C116" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D116">
         <v>1400</v>
@@ -4335,15 +4335,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>112</v>
       </c>
       <c r="B117" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C117" t="s">
-        <v>77</v>
+        <v>181</v>
       </c>
       <c r="D117">
         <v>1500</v>
@@ -4361,15 +4361,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>113</v>
       </c>
       <c r="B118" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C118" t="s">
-        <v>77</v>
+        <v>181</v>
       </c>
       <c r="D118">
         <v>1500</v>
@@ -4387,15 +4387,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>114</v>
       </c>
       <c r="B119" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C119" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D119">
         <v>1600</v>
@@ -4413,15 +4413,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>115</v>
       </c>
       <c r="B120" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C120" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D120">
         <v>1700</v>
@@ -4439,15 +4439,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>116</v>
       </c>
       <c r="B121" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C121" t="s">
-        <v>78</v>
+        <v>182</v>
       </c>
       <c r="D121">
         <v>1800</v>
@@ -4465,15 +4465,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>117</v>
       </c>
       <c r="B122" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C122" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D122">
         <v>1900</v>
@@ -4491,15 +4491,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>118</v>
       </c>
       <c r="B123" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C123" t="s">
-        <v>86</v>
+        <v>190</v>
       </c>
       <c r="D123">
         <v>2000</v>
@@ -4517,15 +4517,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>119</v>
       </c>
       <c r="B124" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C124" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D124">
         <v>2100</v>
@@ -4543,15 +4543,15 @@
         <v>68</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>120</v>
       </c>
       <c r="B125" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C125" t="s">
-        <v>78</v>
+        <v>182</v>
       </c>
       <c r="D125">
         <v>2200</v>
@@ -4569,15 +4569,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>121</v>
       </c>
       <c r="B126" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C126" t="s">
-        <v>78</v>
+        <v>182</v>
       </c>
       <c r="D126">
         <v>2300</v>
@@ -4595,15 +4595,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>122</v>
       </c>
       <c r="B127" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C127" t="s">
-        <v>77</v>
+        <v>181</v>
       </c>
       <c r="D127">
         <v>2400</v>
@@ -4621,15 +4621,15 @@
         <v>62</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>123</v>
       </c>
       <c r="B128" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C128" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D128">
         <v>2500</v>
@@ -4647,15 +4647,15 @@
         <v>67</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>124</v>
       </c>
       <c r="B129" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C129" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D129">
         <v>2600</v>
@@ -4673,15 +4673,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>125</v>
       </c>
       <c r="B130" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C130" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D130">
         <v>2700</v>
@@ -4699,15 +4699,15 @@
         <v>71</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>126</v>
       </c>
       <c r="B131" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C131" t="s">
-        <v>78</v>
+        <v>182</v>
       </c>
       <c r="D131">
         <v>2800</v>
@@ -4725,15 +4725,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>127</v>
       </c>
       <c r="B132" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C132" t="s">
-        <v>85</v>
+        <v>189</v>
       </c>
       <c r="D132">
         <v>2900</v>
@@ -4751,15 +4751,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>128</v>
       </c>
       <c r="B133" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C133" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D133">
         <v>3000</v>
@@ -4777,15 +4777,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>129</v>
       </c>
       <c r="B134" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C134" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D134">
         <v>3100</v>
@@ -4803,15 +4803,15 @@
         <v>64</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>130</v>
       </c>
       <c r="B135" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C135" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
       <c r="D135">
         <v>3200</v>
@@ -4829,15 +4829,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>131</v>
       </c>
       <c r="B136" t="s">
-        <v>242</v>
+        <v>105</v>
       </c>
       <c r="C136" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D136">
         <v>3300</v>
@@ -4855,15 +4855,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>132</v>
       </c>
       <c r="B137" t="s">
-        <v>243</v>
+        <v>106</v>
       </c>
       <c r="C137" t="s">
-        <v>81</v>
+        <v>185</v>
       </c>
       <c r="D137">
         <v>400</v>
@@ -4881,15 +4881,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>133</v>
       </c>
       <c r="B138" t="s">
-        <v>244</v>
+        <v>107</v>
       </c>
       <c r="C138" t="s">
-        <v>80</v>
+        <v>184</v>
       </c>
       <c r="D138">
         <v>5000</v>
@@ -4904,18 +4904,18 @@
         <v>0</v>
       </c>
       <c r="H138" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>134</v>
       </c>
       <c r="B139" t="s">
-        <v>245</v>
+        <v>22</v>
       </c>
       <c r="C139" t="s">
-        <v>80</v>
+        <v>184</v>
       </c>
       <c r="D139">
         <v>5000</v>
@@ -4930,18 +4930,18 @@
         <v>0</v>
       </c>
       <c r="H139" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>135</v>
       </c>
       <c r="B140" t="s">
-        <v>207</v>
+        <v>73</v>
       </c>
       <c r="C140" t="s">
-        <v>79</v>
+        <v>183</v>
       </c>
       <c r="D140">
         <v>1000</v>
@@ -4959,15 +4959,15 @@
         <v>64</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>136</v>
       </c>
       <c r="B141" t="s">
-        <v>246</v>
+        <v>108</v>
       </c>
       <c r="C141" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D141">
         <v>0</v>
@@ -4985,15 +4985,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>137</v>
       </c>
       <c r="B142" t="s">
-        <v>246</v>
+        <v>108</v>
       </c>
       <c r="C142" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="D142">
         <v>0</v>
@@ -5011,15 +5011,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>138</v>
       </c>
       <c r="B143" t="s">
-        <v>246</v>
+        <v>108</v>
       </c>
       <c r="C143" t="s">
-        <v>77</v>
+        <v>181</v>
       </c>
       <c r="D143">
         <v>0</v>
@@ -5037,15 +5037,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>139</v>
       </c>
       <c r="B144" t="s">
-        <v>246</v>
+        <v>108</v>
       </c>
       <c r="C144" t="s">
-        <v>78</v>
+        <v>182</v>
       </c>
       <c r="D144">
         <v>0</v>
@@ -5060,7 +5060,7 @@
         <v>0</v>
       </c>
       <c r="H144" s="2" t="s">
-        <v>139</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>